<commit_message>
Table 1 now readable with behaving format
</commit_message>
<xml_diff>
--- a/Table_raw/relevant_scales.xlsx
+++ b/Table_raw/relevant_scales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://monashuni-my.sharepoint.com/personal/mushfiqul_anwarsiraji_monash_edu/Documents/My papers/LEBA Common workplace/leba-manuscript/Table_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{602B3E3C-C309-704A-89DA-A31EA9AA06C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{602B3E3C-C309-704A-89DA-A31EA9AA06C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D80B5AD-8836-2A4F-B7F1-61118F5220A4}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="2880" windowWidth="28040" windowHeight="17440" xr2:uid="{9797D477-FD80-C04C-AAA6-FBF2673FDC50}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{9797D477-FD80-C04C-AAA6-FBF2673FDC50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Relevant Items</t>
   </si>
   <si>
-    <t>Adaptations</t>
-  </si>
-  <si>
     <t>Visual Light Sensitivity Questionnaire-8</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Eight-question survey to assess the presence and severity of photosensitivity symptoms</t>
   </si>
   <si>
-    <t>Multi-item questionnaire to assess electrical lighting environment in office</t>
-  </si>
-  <si>
     <t>Self-administered semi-quantitative light questionnaire</t>
   </si>
   <si>
@@ -102,49 +96,52 @@
     <t>9 items inventory to measure sleep quality and sleeping pattern</t>
   </si>
   <si>
-    <t>items questionnaire assessing four dimensions of biological rhythm disorder in adolescents (digital media use, sleep, eating habits, and activity)</t>
-  </si>
-  <si>
-    <t>dichotomous (yes/no) items questionnaire to assess "photophobia" and "photophilia", giving two final scores of "photophobic" and "photophilic" behaviours</t>
-  </si>
-  <si>
-    <t>items questionnaire measuring your sleep environment quality</t>
-  </si>
-  <si>
     <t>Item 3,22-25 and 29</t>
   </si>
   <si>
     <t>All itms</t>
   </si>
   <si>
-    <t>[@verriotto2017new]</t>
-  </si>
-  <si>
-    <t>[@eklund1996development]</t>
-  </si>
-  <si>
-    <t>[@bajaj2011validation]</t>
-  </si>
-  <si>
-    <t>[@dianat2013objective]</t>
-  </si>
-  <si>
-    <t>[@horne1976self]</t>
-  </si>
-  <si>
-    <t>[@roenneberg2003life]</t>
-  </si>
-  <si>
-    <t>[@Olivier.2016] | 13</t>
-  </si>
-  <si>
-    <t>[@buysse1989pittsburgh]</t>
-  </si>
-  <si>
-    <t>[@Xie.2021] | 29</t>
-  </si>
-  <si>
-    <t>[@Wu.2017] | 16</t>
+    <t>A survey to assess electrical lighting environment in office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 Items questionnaire assessing four dimensions of biological rhythm disorder in adolescents </t>
+  </si>
+  <si>
+    <t>13 items questionnaire measuring your sleep environment quality</t>
+  </si>
+  <si>
+    <t>16 dichotomous (yes/no) items questionnaire to assess "photophobia" and "photophilia"</t>
+  </si>
+  <si>
+    <t>Verriotto et al., 2017</t>
+  </si>
+  <si>
+    <t>Eklundet al., 1996</t>
+  </si>
+  <si>
+    <t>Bajaj et al., 2011</t>
+  </si>
+  <si>
+    <t>Dianat et el.,.2013</t>
+  </si>
+  <si>
+    <t>Horne et al.,1976</t>
+  </si>
+  <si>
+    <t>Roenneberg et al.,2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olivier et.al.,.2016] </t>
+  </si>
+  <si>
+    <t>Buysse ei al.,1989</t>
+  </si>
+  <si>
+    <t>Xie et al.,2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wu et al.,2017 </t>
   </si>
 </sst>
 </file>
@@ -180,8 +177,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,150 +499,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE174FD3-1659-894F-877B-8FADDCA95335}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="136.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* table 1 updated
</commit_message>
<xml_diff>
--- a/Table_raw/relevant_scales.xlsx
+++ b/Table_raw/relevant_scales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://monashuni-my.sharepoint.com/personal/mushfiqul_anwarsiraji_monash_edu/Documents/My papers/LEBA Common workplace/leba-manuscript/Table_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{602B3E3C-C309-704A-89DA-A31EA9AA06C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00A17FF6-7E43-2E45-94EF-64B85D753914}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{602B3E3C-C309-704A-89DA-A31EA9AA06C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1ABEEDE7-BC8B-724A-861C-2AD20F6D17E3}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="38400" windowHeight="19540" xr2:uid="{9797D477-FD80-C04C-AAA6-FBF2673FDC50}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19540" xr2:uid="{9797D477-FD80-C04C-AAA6-FBF2673FDC50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Relevant Items</t>
-  </si>
-  <si>
     <t>Visual Light Sensitivity Questionnaire-8</t>
   </si>
   <si>
@@ -66,24 +63,15 @@
     <t>Munich Chronotype Questionnaire (MCTQ)</t>
   </si>
   <si>
-    <t>Assessment of Sleep Environment</t>
-  </si>
-  <si>
     <t>The Pittsburgh Sleep Quality Index (PSQI)</t>
   </si>
   <si>
-    <t>Self-Rating of Biological Rhythm Disorder for Adolescents (SBRDA)</t>
-  </si>
-  <si>
     <t>Photosensitivity Assessment Questionnaire (PAQ)</t>
   </si>
   <si>
     <t>Eight-question survey to assess the presence and severity of photosensitivity symptoms</t>
   </si>
   <si>
-    <t>Self-administered semi-quantitative light questionnaire</t>
-  </si>
-  <si>
     <t>23 items questionnaire to assess light environment in a hospital</t>
   </si>
   <si>
@@ -96,21 +84,12 @@
     <t>9 items inventory to measure sleep quality and sleeping pattern</t>
   </si>
   <si>
-    <t>Item 3,22-25 and 29</t>
-  </si>
-  <si>
     <t>All itms</t>
   </si>
   <si>
-    <t>A survey to assess electrical lighting environment in office</t>
-  </si>
-  <si>
     <t xml:space="preserve">29 Items questionnaire assessing four dimensions of biological rhythm disorder in adolescents </t>
   </si>
   <si>
-    <t>13 items questionnaire measuring your sleep environment quality</t>
-  </si>
-  <si>
     <t>16 dichotomous (yes/no) items questionnaire to assess "photophobia" and "photophilia"</t>
   </si>
   <si>
@@ -138,10 +117,97 @@
     <t>Xie et al., 2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Wu et al., 2017 </t>
-  </si>
-  <si>
     <t>Buysse et al., 1989</t>
+  </si>
+  <si>
+    <t>Scale type</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Mixed response format</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Item 29</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Semi-quantitative</t>
+  </si>
+  <si>
+    <t>5-point Likert scale</t>
+  </si>
+  <si>
+    <t>Item 16,17</t>
+  </si>
+  <si>
+    <t>Validity evidences</t>
+  </si>
+  <si>
+    <t>Face and Content validity</t>
+  </si>
+  <si>
+    <t>item 1,2,8,13,14</t>
+  </si>
+  <si>
+    <t>Not available</t>
+  </si>
+  <si>
+    <t>Time spect outdoors</t>
+  </si>
+  <si>
+    <t>30 items survey to assess electrical lighting environment in office</t>
+  </si>
+  <si>
+    <t>1 item semi-quantitative light questionnaire</t>
+  </si>
+  <si>
+    <t> Sleep Practices and Attitudes Questionnaire (SPAQ)</t>
+  </si>
+  <si>
+    <t>Self-Rating of Biological Rhythm Disorder for Disorder for Adolescents (SBRDA)</t>
+  </si>
+  <si>
+    <t>16 Factor questionnaire measuring practice, behavior and attitude related sleep</t>
+  </si>
+  <si>
+    <t>Subscale 8&amp;9</t>
+  </si>
+  <si>
+    <t>Face and Construct validity</t>
+  </si>
+  <si>
+    <t>item 1-4</t>
+  </si>
+  <si>
+    <t>Construct validity</t>
+  </si>
+  <si>
+    <t>Item 3,6,22-25 and 29</t>
+  </si>
+  <si>
+    <t>Binary response option</t>
+  </si>
+  <si>
+    <t>Bossini et al.,2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relevant Items </t>
+  </si>
+  <si>
+    <t>Correlation the oral temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correlation with sleep-logs, actimetry, and physiological parameters </t>
+  </si>
+  <si>
+    <t>Correlation  with clinical measurements</t>
+  </si>
+  <si>
+    <t>Correlation with physical measuremernt</t>
   </si>
 </sst>
 </file>
@@ -177,13 +243,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,21 +562,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE174FD3-1659-894F-877B-8FADDCA95335}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="67.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,123 +589,213 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Table 1 is nor landscape; dpi is set to 300 for all images
</commit_message>
<xml_diff>
--- a/Table_raw/relevant_scales.xlsx
+++ b/Table_raw/relevant_scales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://monashuni-my.sharepoint.com/personal/mushfiqul_anwarsiraji_monash_edu/Documents/My papers/LEBA Common workplace/leba-manuscript/Table_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="8_{602B3E3C-C309-704A-89DA-A31EA9AA06C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85566F56-2DB7-BD44-9223-BA9FEDB183EF}"/>
+  <xr:revisionPtr revIDLastSave="244" documentId="8_{602B3E3C-C309-704A-89DA-A31EA9AA06C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCCBFE8A-E9A0-BC4B-B013-53E03DFFA08D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19540" xr2:uid="{9797D477-FD80-C04C-AAA6-FBF2673FDC50}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -211,10 +211,43 @@
     <t>All items</t>
   </si>
   <si>
-    <t>Self-Rating of Biological Rhythm Disorder for Disorder for\nAdolescents (SBRDA)</t>
-  </si>
-  <si>
-    <t>Visual\nLight Sensitivity Questionnaire-8</t>
+    <t>Visual Light Sensitivity  Questionnaire-8</t>
+  </si>
+  <si>
+    <t>The Pittsburgh Sleep Quality  Index (PSQI)</t>
+  </si>
+  <si>
+    <t>Self-Rating of Biological Rhythm Disorder for Disorder for  Adolescents (SBRDA)</t>
+  </si>
+  <si>
+    <t>Eight-question survey  to assess the  presence and severity of photosensitivity symptoms</t>
+  </si>
+  <si>
+    <t>30 items survey  to assess electrical lighting environment in office</t>
+  </si>
+  <si>
+    <t>23 items questionnaire to assess light environment  in a hospital</t>
+  </si>
+  <si>
+    <t>17 items questionnaire to understand individuals  phase of  entrainment</t>
+  </si>
+  <si>
+    <t>16 Factor questionnaire measuring  practice, behavior and attitude  related sleep</t>
+  </si>
+  <si>
+    <t>9 items inventory  to measure sleep  quality and sleeping pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 Items questionnaire  assessing four  dimensions of biological rhythm  disorder in adolescents </t>
+  </si>
+  <si>
+    <t>16 dichotomous items  questionnaire to assess  "photophobia" and "photophilia"</t>
+  </si>
+  <si>
+    <t>Correlation with oral temperature</t>
+  </si>
+  <si>
+    <t>Correlation  with  clinical measurements</t>
   </si>
 </sst>
 </file>
@@ -571,13 +604,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE174FD3-1659-894F-877B-8FADDCA95335}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="67.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
@@ -607,13 +640,13 @@
     </row>
     <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -633,7 +666,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -673,7 +706,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -702,7 +735,7 @@
         <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -713,7 +746,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
         <v>39</v>
@@ -733,7 +766,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
         <v>45</v>
@@ -747,13 +780,13 @@
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
         <v>47</v>
@@ -762,18 +795,18 @@
         <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
         <v>49</v>
@@ -793,7 +826,7 @@
         <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
         <v>57</v>

</xml_diff>